<commit_message>
Added more books and HTTP links to book_data.xlsx
</commit_message>
<xml_diff>
--- a/data/external/book_data.xlsx
+++ b/data/external/book_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\bachelors_paper_proof_of_concept\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\bachelors_paper_proof_of_concept\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1393DE80-A4BA-4AFE-8467-C35CCAD483CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBCFD75-9816-46E9-BD70-E7731A1BB907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
   <si>
     <t>http</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Victoria Rowe Holbrook</t>
   </si>
   <si>
-    <t>translator_primary_source</t>
-  </si>
-  <si>
-    <t>translator_secondary_source</t>
-  </si>
-  <si>
     <t>Ekin Oklap</t>
   </si>
   <si>
@@ -175,13 +169,193 @@
   </si>
   <si>
     <t>Güneli Gün</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/157993</t>
+  </si>
+  <si>
+    <t>The Little Prince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antoine de Saint-Exupéry, </t>
+  </si>
+  <si>
+    <t>Richard Howard</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/52036</t>
+  </si>
+  <si>
+    <t>Siddharta</t>
+  </si>
+  <si>
+    <t>Hermann Hesse</t>
+  </si>
+  <si>
+    <t>Hilda Rosner</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/16631</t>
+  </si>
+  <si>
+    <t>Steppenwolf</t>
+  </si>
+  <si>
+    <t>Basil Creighton</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/117833</t>
+  </si>
+  <si>
+    <t>The Master and Margarita</t>
+  </si>
+  <si>
+    <t>Mikhail Bulgakov</t>
+  </si>
+  <si>
+    <t>Katherine Tiernan O'Connor</t>
+  </si>
+  <si>
+    <t>translator_first</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/16640</t>
+  </si>
+  <si>
+    <t>The Sorrows of Young Werther</t>
+  </si>
+  <si>
+    <t>R. Dillon Boylan</t>
+  </si>
+  <si>
+    <t>Johann Wolfgang von Goethe</t>
+  </si>
+  <si>
+    <t>The Trial</t>
+  </si>
+  <si>
+    <t>Franz Kafka</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/17690</t>
+  </si>
+  <si>
+    <t>Willa Muir</t>
+  </si>
+  <si>
+    <t>The Stranger</t>
+  </si>
+  <si>
+    <t>Albert Camus</t>
+  </si>
+  <si>
+    <t>Matthew Ward</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/49552</t>
+  </si>
+  <si>
+    <t>Crime and Punishment</t>
+  </si>
+  <si>
+    <t>Fyodor Dostoyevsky</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/7144</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/320</t>
+  </si>
+  <si>
+    <t>One Hundred Years of Solitude</t>
+  </si>
+  <si>
+    <t>Gabriel Garcia Marquez</t>
+  </si>
+  <si>
+    <t>Gregory Rabassa</t>
+  </si>
+  <si>
+    <t>David McDuff</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/527756</t>
+  </si>
+  <si>
+    <t>The Man Without Qualities</t>
+  </si>
+  <si>
+    <t>Robert Musil</t>
+  </si>
+  <si>
+    <t>Sophie Wilkins</t>
+  </si>
+  <si>
+    <t>h10</t>
+  </si>
+  <si>
+    <t>h11</t>
+  </si>
+  <si>
+    <t>h12</t>
+  </si>
+  <si>
+    <t>h13</t>
+  </si>
+  <si>
+    <t>h14</t>
+  </si>
+  <si>
+    <t>h15</t>
+  </si>
+  <si>
+    <t>h16</t>
+  </si>
+  <si>
+    <t>h17</t>
+  </si>
+  <si>
+    <t>h18</t>
+  </si>
+  <si>
+    <t>h19</t>
+  </si>
+  <si>
+    <t>b10</t>
+  </si>
+  <si>
+    <t>b11</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>b13</t>
+  </si>
+  <si>
+    <t>b14</t>
+  </si>
+  <si>
+    <t>b15</t>
+  </si>
+  <si>
+    <t>b16</t>
+  </si>
+  <si>
+    <t>b17</t>
+  </si>
+  <si>
+    <t>b18</t>
+  </si>
+  <si>
+    <t>b19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +376,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,14 +412,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,260 +704,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="C11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -781,7 +1134,17 @@
     <hyperlink ref="B8" r:id="rId7" xr:uid="{D282A5B7-F8F4-446E-BFA4-972DCB81B58C}"/>
     <hyperlink ref="B9" r:id="rId8" xr:uid="{26CA34AA-8551-4FDA-A346-79D3C083992D}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{72FB1D61-0F9D-4705-BDC3-8E5D60E863F3}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{5954817E-BE02-4E1A-8C57-82B6AF07CEE2}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{F4DED667-8F9D-4042-AE9A-F56EF7CF2AB6}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{B53AED72-E84C-4E2E-BBE2-B60C1EBB6F80}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{FAB91D8B-B4C1-4D18-A40E-8458FEC70FC1}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{A6834D0A-5BC5-4F9F-BF47-05A6773B9A30}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{D547696D-C80D-483D-8450-594329B01E9B}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{6137B346-D334-4B5F-BA68-74835140C59F}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{0350EED7-0846-4FDE-AC88-8F2E79513C0A}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{22BAC466-A4DE-494E-91D7-4653EB0FFDE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initialized test_book_data_data_quality.py and added it to dodo.py
</commit_message>
<xml_diff>
--- a/data/external/book_data.xlsx
+++ b/data/external/book_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\bachelors_paper_proof_of_concept\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBCFD75-9816-46E9-BD70-E7731A1BB907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7B2591-52E2-4C46-AA1C-FFAFC4BFAB87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>